<commit_message>
Added sizing data for #101
</commit_message>
<xml_diff>
--- a/examples/case_study_4_fullHVAC/HVAC_sizing_parameter.xlsx
+++ b/examples/case_study_4_fullHVAC/HVAC_sizing_parameter.xlsx
@@ -632,16 +632,16 @@
   </sheetPr>
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C90" activeCellId="0" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="30.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -1410,7 +1410,7 @@
       <c r="D80" s="7" t="n">
         <v>2.112</v>
       </c>
-      <c r="E80" s="7" t="n">
+      <c r="E80" s="8" t="n">
         <v>2.112</v>
       </c>
       <c r="F80" s="7" t="n">
@@ -1458,7 +1458,7 @@
       <c r="D81" s="7" t="n">
         <v>0.5666</v>
       </c>
-      <c r="E81" s="7" t="n">
+      <c r="E81" s="8" t="n">
         <v>0.5666</v>
       </c>
       <c r="F81" s="7" t="n">
@@ -1506,7 +1506,7 @@
       <c r="D82" s="7" t="n">
         <v>0.7772</v>
       </c>
-      <c r="E82" s="7" t="n">
+      <c r="E82" s="8" t="n">
         <v>0.7772</v>
       </c>
       <c r="F82" s="7" t="n">
@@ -1554,7 +1554,7 @@
       <c r="D83" s="7" t="n">
         <v>0.8287</v>
       </c>
-      <c r="E83" s="7" t="n">
+      <c r="E83" s="8" t="n">
         <v>0.8287</v>
       </c>
       <c r="F83" s="7" t="n">
@@ -1602,7 +1602,7 @@
       <c r="D84" s="7" t="n">
         <v>0.7663</v>
       </c>
-      <c r="E84" s="7" t="n">
+      <c r="E84" s="8" t="n">
         <v>0.7663</v>
       </c>
       <c r="F84" s="7" t="n">
@@ -1739,7 +1739,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7" t="s">
         <v>61</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="D96" s="7" t="n">
         <v>0.739</v>
       </c>
-      <c r="E96" s="7" t="n">
+      <c r="E96" s="8" t="n">
         <v>0.739</v>
       </c>
       <c r="F96" s="7" t="n">
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="7" t="s">
         <v>62</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="D97" s="7" t="n">
         <v>0.17</v>
       </c>
-      <c r="E97" s="7" t="n">
+      <c r="E97" s="8" t="n">
         <v>0.17</v>
       </c>
       <c r="F97" s="7" t="n">
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7" t="s">
         <v>63</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="D98" s="7" t="n">
         <v>0.2332</v>
       </c>
-      <c r="E98" s="7" t="n">
+      <c r="E98" s="8" t="n">
         <v>0.2332</v>
       </c>
       <c r="F98" s="7" t="n">
@@ -1871,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="7" t="s">
         <v>64</v>
       </c>
@@ -1884,7 +1884,7 @@
       <c r="D99" s="7" t="n">
         <v>0.2486</v>
       </c>
-      <c r="E99" s="7" t="n">
+      <c r="E99" s="8" t="n">
         <v>0.2486</v>
       </c>
       <c r="F99" s="7" t="n">
@@ -1915,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="7" t="s">
         <v>65</v>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="D100" s="7" t="n">
         <v>0.2299</v>
       </c>
-      <c r="E100" s="7" t="n">
+      <c r="E100" s="8" t="n">
         <v>0.2299</v>
       </c>
       <c r="F100" s="7" t="n">

</xml_diff>

<commit_message>
update the sizing parameter based on 28C discharge temperature
</commit_message>
<xml_diff>
--- a/examples/case_study_4_fullHVAC/HVAC_sizing_parameter.xlsx
+++ b/examples/case_study_4_fullHVAC/HVAC_sizing_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chen046\Documents\GitHub\OBC\issue101\examples\case_study_4_fullHVAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62920042-D216-4138-967E-B69D14BF3AE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D052C146-7D72-4DFF-9EB2-649AB956277A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21396" windowHeight="14616" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,22 +1061,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="8">
-        <v>2.11</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="C11" s="7">
-        <v>0.35485100000000003</v>
+        <v>0.33142100000000002</v>
       </c>
       <c r="D11" s="7">
-        <v>0.34989799999999999</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="E11" s="7">
-        <v>0.73899300000000001</v>
+        <v>0.76659500000000003</v>
       </c>
       <c r="F11" s="7">
-        <v>7.5100000000000004E-4</v>
+        <v>7.7899999999999996E-4</v>
       </c>
       <c r="G11" s="7">
-        <v>0.34989799999999999</v>
+        <v>0.33900000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="36" x14ac:dyDescent="0.3">
@@ -1084,22 +1084,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="8">
-        <v>0.56664099999999995</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="7">
-        <v>0.27882099999999999</v>
+        <v>0.14306099999999999</v>
       </c>
       <c r="D12" s="7">
-        <v>0.3</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="E12" s="7">
-        <v>0.169992</v>
+        <v>0.33572800000000003</v>
       </c>
       <c r="F12" s="7">
-        <v>8.1999999999999998E-4</v>
+        <v>1.619E-3</v>
       </c>
       <c r="G12" s="7">
-        <v>0.3</v>
+        <v>0.30399999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="36" x14ac:dyDescent="0.3">
@@ -1107,22 +1107,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="8">
-        <v>0.77720500000000003</v>
+        <v>0.789493</v>
       </c>
       <c r="C13" s="7">
-        <v>0.128694</v>
+        <v>0.126691</v>
       </c>
       <c r="D13" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E13" s="7">
-        <v>0.23316100000000001</v>
+        <v>0.15789900000000001</v>
       </c>
       <c r="F13" s="7">
-        <v>1.776E-3</v>
+        <v>1.2030000000000001E-3</v>
       </c>
       <c r="G13" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="36" x14ac:dyDescent="0.3">
@@ -1130,22 +1130,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="8">
-        <v>0.82867599999999997</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C14" s="7">
-        <v>0.19065599999999999</v>
+        <v>0.14118700000000001</v>
       </c>
       <c r="D14" s="7">
-        <v>0.3</v>
+        <v>0.249</v>
       </c>
       <c r="E14" s="7">
-        <v>0.24860299999999999</v>
+        <v>0.27863700000000002</v>
       </c>
       <c r="F14" s="7">
-        <v>1.199E-3</v>
+        <v>1.3439999999999999E-3</v>
       </c>
       <c r="G14" s="7">
-        <v>0.3</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="36" x14ac:dyDescent="0.3">
@@ -1153,21 +1153,23 @@
         <v>13</v>
       </c>
       <c r="B15" s="8">
-        <v>0.76634899999999995</v>
+        <v>0.790601</v>
       </c>
       <c r="C15" s="7">
-        <v>0.13050899999999999</v>
+        <v>0.12650500000000001</v>
       </c>
       <c r="D15" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E15" s="7">
-        <v>0.229905</v>
+        <v>0.15812000000000001</v>
       </c>
       <c r="F15" s="7">
-        <v>1.7520000000000001E-3</v>
-      </c>
-      <c r="G15" s="9"/>
+        <v>1.2049999999999999E-3</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -1188,39 +1190,39 @@
         <v>16</v>
       </c>
       <c r="B22" s="8">
-        <v>24101.91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+        <v>31889.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="8">
-        <v>12755.56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+        <v>20127.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="8">
-        <v>8391.1200000000008</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+        <v>13248.64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="8">
-        <v>12928.79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+        <v>20395.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="8">
-        <v>8505.89</v>
+        <v>13414.6</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1266,31 +1268,31 @@
         <v>31</v>
       </c>
       <c r="B33" s="7">
-        <v>1.62</v>
+        <v>1.7</v>
       </c>
       <c r="C33" s="7">
-        <v>1.62</v>
+        <v>1.7</v>
       </c>
       <c r="D33" s="7">
-        <v>5.05</v>
+        <v>6.06</v>
       </c>
       <c r="E33" s="7">
-        <v>1.9</v>
+        <v>5.44</v>
       </c>
       <c r="F33" s="7">
-        <v>4.32</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="G33" s="7">
-        <v>4.32</v>
+        <v>5.44</v>
       </c>
       <c r="H33" s="7">
         <v>0.3</v>
       </c>
       <c r="I33" s="7">
-        <v>0.43873099999999998</v>
+        <v>1</v>
       </c>
       <c r="J33" s="8">
-        <v>4.32</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.35">
@@ -1317,7 +1319,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="7">
-        <v>4.32</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="18" x14ac:dyDescent="0.35">
@@ -1357,22 +1359,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="7">
-        <v>4.32</v>
+        <v>5.44</v>
       </c>
       <c r="C44" s="7">
-        <v>102700.15</v>
+        <v>128026.53</v>
       </c>
       <c r="D44" s="7">
-        <v>0.71502600000000005</v>
+        <v>0.71741200000000005</v>
       </c>
       <c r="E44" s="7">
-        <v>1.44</v>
+        <v>1.81</v>
       </c>
       <c r="F44" s="7">
-        <v>34229.96</v>
+        <v>42671.24</v>
       </c>
       <c r="G44" s="7">
-        <v>0.69</v>
+        <v>0.71741200000000005</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="18" x14ac:dyDescent="0.35">
@@ -1399,7 +1401,7 @@
         <v>45</v>
       </c>
       <c r="B50" s="7">
-        <v>45601.18</v>
+        <v>43895.519999999997</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.35">
@@ -1426,7 +1428,7 @@
         <v>48</v>
       </c>
       <c r="B56" s="7">
-        <v>4.32</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.35">
@@ -1489,7 +1491,7 @@
         <v>31</v>
       </c>
       <c r="C69" s="7">
-        <v>23.02</v>
+        <v>21.84</v>
       </c>
       <c r="D69" s="7">
         <v>52.94</v>
@@ -1515,7 +1517,7 @@
         <v>31</v>
       </c>
       <c r="C70" s="7">
-        <v>4.8499999999999996</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="D70" s="7">
         <v>11.16</v>
@@ -1541,7 +1543,7 @@
         <v>31</v>
       </c>
       <c r="C71" s="7">
-        <v>3.07</v>
+        <v>2.56</v>
       </c>
       <c r="D71" s="7">
         <v>7.07</v>
@@ -1567,7 +1569,7 @@
         <v>31</v>
       </c>
       <c r="C72" s="7">
-        <v>4.8499999999999996</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="D72" s="7">
         <v>11.16</v>
@@ -1593,7 +1595,7 @@
         <v>31</v>
       </c>
       <c r="C73" s="7">
-        <v>3.07</v>
+        <v>2.92</v>
       </c>
       <c r="D73" s="7">
         <v>7.06</v>
@@ -1672,13 +1674,13 @@
         <v>79</v>
       </c>
       <c r="D80" s="7">
-        <v>2.1120000000000001</v>
+        <v>2.2612999999999999</v>
       </c>
       <c r="E80" s="8">
-        <v>2.113</v>
+        <v>2.2612999999999999</v>
       </c>
       <c r="F80" s="15">
-        <v>0.73899999999999999</v>
+        <v>0.76659999999999995</v>
       </c>
       <c r="G80" s="7">
         <v>0</v>
@@ -1706,7 +1708,7 @@
       </c>
       <c r="O80">
         <f>F80/E80</f>
-        <v>0.34973970657832465</v>
+        <v>0.33900853491354532</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="36" x14ac:dyDescent="0.3">
@@ -1720,13 +1722,13 @@
         <v>79</v>
       </c>
       <c r="D81" s="7">
-        <v>0.56659999999999999</v>
+        <v>1.1285000000000001</v>
       </c>
       <c r="E81" s="8">
-        <v>0.56659999999999999</v>
+        <v>1.1285000000000001</v>
       </c>
       <c r="F81" s="15">
-        <v>0.17</v>
+        <v>0.40629999999999999</v>
       </c>
       <c r="G81" s="7">
         <v>0</v>
@@ -1754,7 +1756,7 @@
       </c>
       <c r="O81">
         <f>F81/E81</f>
-        <v>0.30003529827038478</v>
+        <v>0.3600354452813469</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="36" x14ac:dyDescent="0.3">
@@ -1768,13 +1770,13 @@
         <v>79</v>
       </c>
       <c r="D82" s="7">
-        <v>0.7772</v>
+        <v>0.74139999999999995</v>
       </c>
       <c r="E82" s="8">
-        <v>0.7772</v>
+        <v>0.74139999999999995</v>
       </c>
       <c r="F82" s="15">
-        <v>0.23319999999999999</v>
+        <v>0.14829999999999999</v>
       </c>
       <c r="G82" s="7">
         <v>0</v>
@@ -1802,7 +1804,7 @@
       </c>
       <c r="O82">
         <f>F82/E82</f>
-        <v>0.30005146680391148</v>
+        <v>0.20002697599136768</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="36" x14ac:dyDescent="0.3">
@@ -1816,13 +1818,13 @@
         <v>79</v>
       </c>
       <c r="D83" s="7">
-        <v>0.82869999999999999</v>
+        <v>1.139</v>
       </c>
       <c r="E83" s="8">
-        <v>0.82869999999999999</v>
+        <v>1.139</v>
       </c>
       <c r="F83" s="15">
-        <v>0.24859999999999999</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="G83" s="7">
         <v>0</v>
@@ -1850,7 +1852,7 @@
       </c>
       <c r="O83">
         <f>F83/E83</f>
-        <v>0.29998793290696268</v>
+        <v>0.30904302019315188</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="36" x14ac:dyDescent="0.3">
@@ -1864,13 +1866,13 @@
         <v>79</v>
       </c>
       <c r="D84" s="7">
-        <v>0.76629999999999998</v>
+        <v>0.75009999999999999</v>
       </c>
       <c r="E84" s="8">
-        <v>0.76629999999999998</v>
+        <v>0.75009999999999999</v>
       </c>
       <c r="F84" s="15">
-        <v>0.22989999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="G84" s="7">
         <v>0</v>
@@ -1898,7 +1900,7 @@
       </c>
       <c r="O84">
         <f>F84/E84</f>
-        <v>0.30001304971943105</v>
+        <v>0.19997333688841487</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1935,16 +1937,16 @@
         <v>31</v>
       </c>
       <c r="B90" s="7">
-        <v>5.0509000000000004</v>
+        <v>6.0648</v>
       </c>
       <c r="C90" s="15">
-        <v>4.3204000000000002</v>
+        <v>4.5202</v>
       </c>
       <c r="D90" s="7">
-        <v>5.0509000000000004</v>
+        <v>6.0648</v>
       </c>
       <c r="E90" s="7">
-        <v>1.6207</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="F90" s="7">
         <v>0</v>
@@ -2014,13 +2016,13 @@
         <v>79</v>
       </c>
       <c r="D96" s="7">
-        <v>0.73899999999999999</v>
+        <v>0.76659999999999995</v>
       </c>
       <c r="E96" s="8">
-        <v>0.73899999999999999</v>
+        <v>0.76659999999999995</v>
       </c>
       <c r="F96" s="7">
-        <v>0.73899999999999999</v>
+        <v>0.76659999999999995</v>
       </c>
       <c r="G96" s="7">
         <v>0</v>
@@ -2058,13 +2060,13 @@
         <v>79</v>
       </c>
       <c r="D97" s="7">
-        <v>0.17</v>
+        <v>0.3357</v>
       </c>
       <c r="E97" s="8">
-        <v>0.17</v>
+        <v>0.3357</v>
       </c>
       <c r="F97" s="7">
-        <v>0.17</v>
+        <v>0.3357</v>
       </c>
       <c r="G97" s="7">
         <v>0</v>
@@ -2102,13 +2104,13 @@
         <v>79</v>
       </c>
       <c r="D98" s="7">
-        <v>0.23319999999999999</v>
+        <v>0.15790000000000001</v>
       </c>
       <c r="E98" s="8">
-        <v>0.23319999999999999</v>
+        <v>0.15790000000000001</v>
       </c>
       <c r="F98" s="7">
-        <v>0.23319999999999999</v>
+        <v>0.15790000000000001</v>
       </c>
       <c r="G98" s="7">
         <v>0</v>
@@ -2146,13 +2148,13 @@
         <v>79</v>
       </c>
       <c r="D99" s="7">
-        <v>0.24859999999999999</v>
+        <v>0.27860000000000001</v>
       </c>
       <c r="E99" s="8">
-        <v>0.24859999999999999</v>
+        <v>0.27860000000000001</v>
       </c>
       <c r="F99" s="7">
-        <v>0.24859999999999999</v>
+        <v>0.27860000000000001</v>
       </c>
       <c r="G99" s="7">
         <v>0</v>
@@ -2190,13 +2192,13 @@
         <v>79</v>
       </c>
       <c r="D100" s="7">
-        <v>0.22989999999999999</v>
+        <v>0.15809999999999999</v>
       </c>
       <c r="E100" s="8">
-        <v>0.22989999999999999</v>
+        <v>0.15809999999999999</v>
       </c>
       <c r="F100" s="7">
-        <v>0.22989999999999999</v>
+        <v>0.15809999999999999</v>
       </c>
       <c r="G100" s="7">
         <v>0</v>
@@ -2257,16 +2259,16 @@
         <v>31</v>
       </c>
       <c r="B106" s="7">
-        <v>1.6207</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="C106" s="15">
-        <v>1.6207</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="D106" s="7">
-        <v>1.6207</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="E106" s="7">
-        <v>1.6207</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="F106" s="7">
         <v>0</v>

</xml_diff>